<commit_message>
Tracker updates, additional ballot files, updated agenda
</commit_message>
<xml_diff>
--- a/Agendas/201805 Cologne WGM FHIR Agenda.xlsx
+++ b/Agendas/201805 Cologne WGM FHIR Agenda.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR-documents\Agendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8883C0C8-05CC-4710-A989-5BFDAE7BD180}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="65">
   <si>
     <t>Mon</t>
   </si>
@@ -212,6 +213,12 @@
   </si>
   <si>
     <t>TSC</t>
+  </si>
+  <si>
+    <t>Reception</t>
+  </si>
+  <si>
+    <t>FHIRCast</t>
   </si>
 </sst>
 </file>
@@ -648,10 +655,10 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,9 +906,13 @@
         <v>26</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -998,7 +1009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1006,6 +1017,9 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">

</xml_diff>

<commit_message>
Jan FHIR agenda, updates to trackers,
</commit_message>
<xml_diff>
--- a/Agendas/201805 Cologne WGM FHIR Agenda.xlsx
+++ b/Agendas/201805 Cologne WGM FHIR Agenda.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR-documents\Agendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8883C0C8-05CC-4710-A989-5BFDAE7BD180}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA25B03A-A2B9-42AC-92D3-32D13D0A0B94}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,13 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>Mon</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Fri</t>
-  </si>
-  <si>
-    <t>Clinical Connectathon</t>
   </si>
   <si>
     <t>CIMI</t>
@@ -225,7 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +257,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -287,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -311,6 +324,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,10 +680,10 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,16 +741,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -733,16 +758,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -770,10 +795,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -783,33 +808,33 @@
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>42</v>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -817,16 +842,16 @@
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -836,22 +861,22 @@
       <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>42</v>
+      <c r="D11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>47</v>
+      <c r="C12" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>20</v>
@@ -874,10 +899,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,13 +913,13 @@
         <v>36</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -907,11 +932,11 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -928,10 +953,10 @@
         <v>14</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -942,16 +967,16 @@
         <v>32</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,16 +984,16 @@
         <v>23</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -980,16 +1005,16 @@
         <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>60</v>
+      <c r="G19" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -997,16 +1022,16 @@
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1018,7 +1043,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1032,7 +1057,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>29</v>
@@ -1040,8 +1065,8 @@
       <c r="F22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>60</v>
+      <c r="G22" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1051,14 +1076,14 @@
       <c r="C23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>42</v>
+      <c r="D23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1066,16 +1091,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1092,7 +1117,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1106,7 +1131,7 @@
         <v>30</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>16</v>
@@ -1120,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>18</v>
@@ -1131,8 +1156,8 @@
       <c r="F27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>60</v>
+      <c r="G27" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1146,10 +1171,10 @@
         <v>16</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1169,10 +1194,10 @@
         <v>20</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,71 +1205,47 @@
         <v>4</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>

</xml_diff>